<commit_message>
Manually compared to recovery file pdf from 2020 sep 27 10:00am
</commit_message>
<xml_diff>
--- a/Z_tables/Keyword_Frequency__zh-en-comparison.xlsx
+++ b/Z_tables/Keyword_Frequency__zh-en-comparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Personal/Academia/My Papers/02 - Papers/2020/JITT/latex-itt/Z_tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/icekler/Local_Github/latex-itt/Z_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139EBFCC-0DDB-2F42-ADAC-049B354687B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7D7BDA-54BC-964B-8DA1-31F6B4A0BC23}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="460" windowWidth="23960" windowHeight="15540" activeTab="1" xr2:uid="{FD04936F-828B-D74C-92A5-055D54B95716}"/>
+    <workbookView xWindow="-19220" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{FD04936F-828B-D74C-92A5-055D54B95716}"/>
   </bookViews>
   <sheets>
     <sheet name="Positive" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="88">
   <si>
     <t>Price range</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>wonderful</t>
+  </si>
+  <si>
+    <t>\begin{CJK}{UTF8}{gbsn}华人\end{CJK} (Chinese)</t>
   </si>
 </sst>
 </file>
@@ -351,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -363,6 +366,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A21480-2FA4-4140-90C7-E3B6B39EE3CF}">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -710,19 +717,19 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="7" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1961,8 +1968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB3382D-CA19-6840-9271-296BB54CFEA0}">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2116,8 +2123,12 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="2">
+        <v>15</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
@@ -2226,8 +2237,12 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2</v>
+      </c>
       <c r="D19" s="2" t="s">
         <v>54</v>
       </c>
@@ -2528,8 +2543,12 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+      <c r="B41" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="2">
+        <v>3</v>
+      </c>
       <c r="D41" s="2" t="s">
         <v>47</v>
       </c>
@@ -2668,8 +2687,12 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="5"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
+      <c r="B51" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C51" s="2">
+        <v>2</v>
+      </c>
       <c r="D51" s="2" t="s">
         <v>45</v>
       </c>
@@ -2808,8 +2831,12 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="5"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
+      <c r="B61" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C61" s="2">
+        <v>2</v>
+      </c>
       <c r="D61" s="2" t="s">
         <v>44</v>
       </c>
@@ -2948,8 +2975,12 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="5"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
+      <c r="B71" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C71" s="2">
+        <v>8</v>
+      </c>
       <c r="D71" s="2" t="s">
         <v>46</v>
       </c>

</xml_diff>